<commit_message>
add ISBN and delete the same folder
just done 1/2, another will be done in this everning
</commit_message>
<xml_diff>
--- a/Documents/Data/Art&Photography/art_photography.xlsx
+++ b/Documents/Data/Art&Photography/art_photography.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
   <si>
     <t>STT</t>
   </si>
@@ -165,9 +165,6 @@
     <t>Michael Ochs</t>
   </si>
   <si>
-    <t>english</t>
-  </si>
-  <si>
     <t>Jacket madness: A splendid collection of album art from the 1960s to the 90s Record covers are a sign of our life and times. Like the music on the discs, they address such issues as love, life, death, fashion, and rebellion. For music fans the covers are the expression of a period, of a particular time in their lives. Many are works of art and have become as famous as the music they stand for Andy Warhol's covers, for example, including the banana he designed for The Velvet Underground.This edition ofRecord Coverspresents a selection of the best rock album covers of the 60s to 90s from music archivist, disc jockey, journalist, and former record-publicity executive Michael Ochs s enormous private collection. Both a trip down memory lane and a study in the evolution of cover art, this is a sweeping look at an underappreciated art form</t>
   </si>
   <si>
@@ -178,6 +175,9 @@
   </si>
   <si>
     <t>Alex Steinweiss invented the album cover as we know it. In 1940, as Columbia Records' young new art director, he pitched an idea: Why not replace the standard plain brown wrapper with an eye-catching illustration? The company took a chance, and within months its record sales increased by over 800 per cent. Over the next three decades, Steinweiss made thousands of original artworks for classical, jazz, and popular record covers for Columbia, Decca, London, and Everest; as well as logos, labels, advertising material, even his own typeface, the Steinweiss Scrawl.</t>
+  </si>
+  <si>
+    <t>ISBN13</t>
   </si>
 </sst>
 </file>
@@ -187,7 +187,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,6 +236,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -258,7 +270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -272,6 +284,13 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -587,25 +606,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="23.109375" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" customWidth="1"/>
-    <col min="8" max="8" width="25.109375" customWidth="1"/>
-    <col min="9" max="9" width="25.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" customWidth="1"/>
+    <col min="10" max="10" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1">
+    <row r="1" spans="1:10" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -621,20 +641,23 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
@@ -650,20 +673,23 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="11">
+        <v>9781471157790</v>
+      </c>
+      <c r="G2" s="3">
         <v>23.03</v>
       </c>
-      <c r="G2" s="4">
+      <c r="H2" s="4">
         <v>42711</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>2</v>
       </c>
@@ -679,20 +705,23 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="11">
+        <v>9781908944191</v>
+      </c>
+      <c r="G3" s="3">
         <v>6.99</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3" s="4">
         <v>41725</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>3</v>
       </c>
@@ -708,20 +737,23 @@
       <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="11">
+        <v>9783836508766</v>
+      </c>
+      <c r="G4" s="3">
         <v>55.5</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="4">
         <v>42694</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>23</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>4</v>
       </c>
@@ -737,20 +769,23 @@
       <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="11">
+        <v>9781579655976</v>
+      </c>
+      <c r="G5" s="3">
         <v>31.55</v>
       </c>
-      <c r="G5" s="4">
+      <c r="H5" s="4">
         <v>42647</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>28</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>5</v>
       </c>
@@ -766,49 +801,55 @@
       <c r="E6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="11">
+        <v>9780500252154</v>
+      </c>
+      <c r="G6" s="3">
         <v>24.87</v>
       </c>
-      <c r="G6" s="4">
+      <c r="H6" s="4">
         <v>42268</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>13</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7">
+    <row r="7" spans="1:10" s="12" customFormat="1">
+      <c r="A7" s="12">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="15">
+        <v>9781780233581</v>
+      </c>
+      <c r="G7" s="13">
         <v>31.98</v>
       </c>
-      <c r="G7" s="4">
+      <c r="H7" s="14">
         <v>42003</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" s="12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>7</v>
       </c>
@@ -824,20 +865,23 @@
       <c r="E8" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="11">
+        <v>9780500517864</v>
+      </c>
+      <c r="G8" s="3">
         <v>40.049999999999997</v>
       </c>
-      <c r="G8" s="4">
+      <c r="H8" s="4">
         <v>42254</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>40</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="27.6">
+    <row r="9" spans="1:10" ht="28.5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -853,20 +897,23 @@
       <c r="E9" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="11">
+        <v>9783836556361</v>
+      </c>
+      <c r="G9" s="3">
         <v>26.3</v>
       </c>
-      <c r="G9" s="4">
+      <c r="H9" s="4">
         <v>42167</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>23</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>9</v>
       </c>
@@ -880,30 +927,33 @@
         <v>22</v>
       </c>
       <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="11">
+        <v>9783836550581</v>
+      </c>
+      <c r="G10" s="3">
+        <v>24.68</v>
+      </c>
+      <c r="H10" s="8">
+        <v>41774</v>
+      </c>
+      <c r="I10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="3">
-        <v>24.68</v>
-      </c>
-      <c r="G10" s="8">
-        <v>41774</v>
-      </c>
-      <c r="H10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="s">
         <v>50</v>
-      </c>
-      <c r="C11" t="s">
-        <v>51</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
@@ -911,17 +961,20 @@
       <c r="E11" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="11">
+        <v>9783836557764</v>
+      </c>
+      <c r="G11" s="3">
         <v>20.62</v>
       </c>
-      <c r="G11" s="4">
+      <c r="H11" s="4">
         <v>42309</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>23</v>
       </c>
-      <c r="I11" t="s">
-        <v>52</v>
+      <c r="J11" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>